<commit_message>
Updated API for players management for auctions
</commit_message>
<xml_diff>
--- a/public/Format/Import Players Format.xlsx
+++ b/public/Format/Import Players Format.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="786">
   <si>
     <t>Full Name</t>
   </si>
@@ -2379,17 +2379,26 @@
     <t>Sultanpur</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>State</t>
+  </si>
+  <si>
+    <t>Player Role</t>
+  </si>
+  <si>
+    <t>Batting Style</t>
+  </si>
+  <si>
+    <t>Bowling Style</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2400,12 +2409,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Consolas"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2457,15 +2460,15 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2684,29 +2687,32 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="36.59765625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="36.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="36.59765625" style="3" customWidth="1"/>
     <col min="6" max="6" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.73046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.265625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="23.265625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="17.86328125" customWidth="1"/>
+    <col min="16" max="16" width="19.53125" customWidth="1"/>
+    <col min="17" max="17" width="14.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2716,10 +2722,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>782</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="8" t="s">
+        <v>781</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -2743,195 +2749,205 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F2" s="7"/>
-      <c r="G2" s="4" t="s">
-        <v>781</v>
-      </c>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F3" s="7"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F4" s="7"/>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F5" s="7"/>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F6" s="7"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F7" s="7"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F8" s="7"/>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F9" s="7"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F10" s="7"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F11" s="7"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F12" s="7"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F13" s="7"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F14" s="7"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F15" s="7"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F16" s="7"/>
-      <c r="K16" s="6"/>
+    <row r="2" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F2" s="6"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F3" s="6"/>
+      <c r="K3" s="5"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F4" s="6"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F5" s="6"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F6" s="6"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F7" s="6"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F8" s="6"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F9" s="6"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F10" s="6"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F11" s="6"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F12" s="6"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F13" s="6"/>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F14" s="6"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F15" s="6"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="F16" s="6"/>
+      <c r="K16" s="5"/>
     </row>
     <row r="17" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F17" s="7"/>
-      <c r="K17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="K17" s="5"/>
     </row>
     <row r="18" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F18" s="7"/>
-      <c r="K18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F19" s="7"/>
-      <c r="K19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F20" s="7"/>
-      <c r="K20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="K20" s="5"/>
     </row>
     <row r="21" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F21" s="7"/>
-      <c r="K21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="K21" s="5"/>
     </row>
     <row r="22" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F22" s="7"/>
-      <c r="K22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="K22" s="5"/>
     </row>
     <row r="23" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F23" s="7"/>
-      <c r="K23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="K23" s="5"/>
     </row>
     <row r="24" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F24" s="7"/>
-      <c r="K24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="K24" s="5"/>
     </row>
     <row r="25" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F25" s="7"/>
-      <c r="K25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="K25" s="5"/>
     </row>
     <row r="26" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F26" s="7"/>
-      <c r="K26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="K26" s="5"/>
     </row>
     <row r="27" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F27" s="7"/>
-      <c r="K27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="K27" s="5"/>
     </row>
     <row r="28" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F28" s="7"/>
-      <c r="K28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="K28" s="5"/>
     </row>
     <row r="29" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F29" s="7"/>
-      <c r="K29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="K29" s="5"/>
     </row>
     <row r="30" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F30" s="7"/>
-      <c r="K30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="K30" s="5"/>
     </row>
     <row r="31" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F31" s="7"/>
-      <c r="K31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="K31" s="5"/>
     </row>
     <row r="32" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F32" s="7"/>
-      <c r="K32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="K32" s="5"/>
     </row>
     <row r="33" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F33" s="7"/>
-      <c r="K33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="K33" s="5"/>
     </row>
     <row r="34" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F34" s="7"/>
-      <c r="K34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="K34" s="5"/>
     </row>
     <row r="35" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F35" s="7"/>
-      <c r="K35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="K35" s="5"/>
     </row>
     <row r="36" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F36" s="7"/>
-      <c r="K36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="K36" s="5"/>
     </row>
     <row r="37" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F37" s="7"/>
-      <c r="K37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="K37" s="5"/>
     </row>
     <row r="38" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F38" s="7"/>
-      <c r="K38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="K38" s="5"/>
     </row>
     <row r="39" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F39" s="7"/>
-      <c r="K39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="K39" s="5"/>
     </row>
     <row r="40" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F40" s="7"/>
-      <c r="K40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="K40" s="5"/>
     </row>
     <row r="41" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F41" s="7"/>
-      <c r="K41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="K41" s="5"/>
     </row>
     <row r="42" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F42" s="7"/>
-      <c r="K42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="K42" s="5"/>
     </row>
     <row r="43" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F43" s="7"/>
-      <c r="K43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="K43" s="5"/>
     </row>
     <row r="44" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F44" s="7"/>
-      <c r="K44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="K44" s="5"/>
     </row>
     <row r="45" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F45" s="7"/>
-      <c r="K45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="K45" s="5"/>
     </row>
     <row r="46" spans="6:11" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="F46" s="7"/>
-      <c r="K46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="K46" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="I2:J46 L2:L46">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
@@ -2940,6 +2956,15 @@
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="C2:C46">
       <formula1>IFERROR(ISEMAIL(C2), TRUE)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5 M2:M1048576">
+      <formula1>"Top-order Batsman, Middle-order Batsman, Bowler, All-rounder, Lower-order Batsman, Opening Batsman, None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576">
+      <formula1>"Left-hand Batsman, Right-hand Batsman"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576">
+      <formula1>"Right-arm fast, Right-arm medium, Left-arm fast, Left-arm medium, Slow left-arm orthodox, Slow left-arm chinaman , Right-arm Off Break, Right-arm Leg Break, None"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3130,2413 +3155,2413 @@
       </c>
     </row>
     <row r="5" spans="3:38" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="N5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="O5" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="Q5" s="8" t="s">
+      <c r="Q5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="R5" s="8" t="s">
+      <c r="R5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="S5" s="8" t="s">
+      <c r="S5" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="T5" s="8" t="s">
+      <c r="T5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="U5" s="8" t="s">
+      <c r="U5" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="V5" s="8" t="s">
+      <c r="V5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="W5" s="8" t="s">
+      <c r="W5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="X5" s="8" t="s">
+      <c r="X5" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="Y5" s="8" t="s">
+      <c r="Y5" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="Z5" s="8" t="s">
+      <c r="Z5" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AA5" s="8" t="s">
+      <c r="AA5" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="AB5" s="8" t="s">
+      <c r="AB5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AC5" s="8" t="s">
+      <c r="AC5" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AD5" s="8" t="s">
+      <c r="AD5" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="AE5" s="8" t="s">
+      <c r="AE5" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="AF5" s="8" t="s">
+      <c r="AF5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AG5" s="8" t="s">
+      <c r="AG5" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="AH5" s="8" t="s">
+      <c r="AH5" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AI5" s="8" t="s">
+      <c r="AI5" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AJ5" s="8" t="s">
+      <c r="AJ5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="AK5" s="8" t="s">
+      <c r="AK5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AL5" s="8" t="s">
+      <c r="AL5" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="6" spans="3:38" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="Q6" s="8" t="s">
+      <c r="Q6" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="R6" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="S6" s="8" t="s">
+      <c r="S6" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="T6" s="8" t="s">
+      <c r="T6" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="U6" s="8" t="s">
+      <c r="U6" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="V6" s="8" t="s">
+      <c r="V6" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="W6" s="8" t="s">
+      <c r="W6" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="X6" s="8" t="s">
+      <c r="X6" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="Y6" s="8" t="s">
+      <c r="Y6" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="Z6" s="8" t="s">
+      <c r="Z6" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="AA6" s="8" t="s">
+      <c r="AA6" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="AB6" s="8" t="s">
+      <c r="AB6" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="AC6" s="8" t="s">
+      <c r="AC6" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="AD6" s="8" t="s">
+      <c r="AD6" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="AE6" s="8" t="s">
+      <c r="AE6" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="AF6" s="8" t="s">
+      <c r="AF6" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="AG6" s="8" t="s">
+      <c r="AG6" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="AH6" s="8" t="s">
+      <c r="AH6" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="AI6" s="8" t="s">
+      <c r="AI6" s="7" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="7" spans="3:38" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="M7" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="N7" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="O7" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="Q7" s="8" t="s">
+      <c r="Q7" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="R7" s="8" t="s">
+      <c r="R7" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="S7" s="8" t="s">
+      <c r="S7" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="T7" s="8" t="s">
+      <c r="T7" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="U7" s="8" t="s">
+      <c r="U7" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="V7" s="8" t="s">
+      <c r="V7" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="W7" s="8" t="s">
+      <c r="W7" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="X7" s="8" t="s">
+      <c r="X7" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="Y7" s="8" t="s">
+      <c r="Y7" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="Z7" s="8" t="s">
+      <c r="Z7" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="AA7" s="8" t="s">
+      <c r="AA7" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="AB7" s="8" t="s">
+      <c r="AB7" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="AC7" s="8" t="s">
+      <c r="AC7" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="AF7" s="8" t="s">
+      <c r="AF7" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="AG7" s="8" t="s">
+      <c r="AG7" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="AH7" s="8" t="s">
+      <c r="AH7" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="AI7" s="8" t="s">
+      <c r="AI7" s="7" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="8" spans="3:38" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="L8" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="M8" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="N8" s="8" t="s">
+      <c r="N8" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="O8" s="8" t="s">
+      <c r="O8" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="P8" s="8" t="s">
+      <c r="P8" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="Q8" s="8" t="s">
+      <c r="Q8" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="R8" s="8" t="s">
+      <c r="R8" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="S8" s="8" t="s">
+      <c r="S8" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="T8" s="8" t="s">
+      <c r="T8" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="U8" s="8" t="s">
+      <c r="U8" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="V8" s="8" t="s">
+      <c r="V8" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="W8" s="8" t="s">
+      <c r="W8" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="X8" s="8" t="s">
+      <c r="X8" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="Y8" s="8" t="s">
+      <c r="Y8" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="Z8" s="8" t="s">
+      <c r="Z8" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="AA8" s="8" t="s">
+      <c r="AA8" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="AB8" s="8" t="s">
+      <c r="AB8" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="AC8" s="8" t="s">
+      <c r="AC8" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="AF8" s="8" t="s">
+      <c r="AF8" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="AH8" s="8" t="s">
+      <c r="AH8" s="7" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="9" spans="3:38" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="L9" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="M9" s="8" t="s">
+      <c r="M9" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="N9" s="8" t="s">
+      <c r="N9" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="O9" s="8" t="s">
+      <c r="O9" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="P9" s="8" t="s">
+      <c r="P9" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="Q9" s="8" t="s">
+      <c r="Q9" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="R9" s="8" t="s">
+      <c r="R9" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="S9" s="8" t="s">
+      <c r="S9" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="T9" s="8" t="s">
+      <c r="T9" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="U9" s="8" t="s">
+      <c r="U9" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="V9" s="8" t="s">
+      <c r="V9" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="W9" s="8" t="s">
+      <c r="W9" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="X9" s="8" t="s">
+      <c r="X9" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="Y9" s="8" t="s">
+      <c r="Y9" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="Z9" s="8" t="s">
+      <c r="Z9" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="AA9" s="8" t="s">
+      <c r="AA9" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="AB9" s="8" t="s">
+      <c r="AB9" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="AC9" s="8" t="s">
+      <c r="AC9" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="AH9" s="8" t="s">
+      <c r="AH9" s="7" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="10" spans="3:38" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="L10" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="M10" s="8" t="s">
+      <c r="M10" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="N10" s="8" t="s">
+      <c r="N10" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="O10" s="8" t="s">
+      <c r="O10" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="P10" s="8" t="s">
+      <c r="P10" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="Q10" s="8" t="s">
+      <c r="Q10" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="R10" s="8" t="s">
+      <c r="R10" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="S10" s="8" t="s">
+      <c r="S10" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="T10" s="8" t="s">
+      <c r="T10" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="U10" s="8" t="s">
+      <c r="U10" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="V10" s="8" t="s">
+      <c r="V10" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="W10" s="8" t="s">
+      <c r="W10" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="X10" s="8" t="s">
+      <c r="X10" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="Y10" s="8" t="s">
+      <c r="Y10" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="Z10" s="8" t="s">
+      <c r="Z10" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="AA10" s="8" t="s">
+      <c r="AA10" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="AB10" s="8" t="s">
+      <c r="AB10" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="AC10" s="8" t="s">
+      <c r="AC10" s="7" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="11" spans="3:38" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="L11" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="M11" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="N11" s="8" t="s">
+      <c r="N11" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="O11" s="8" t="s">
+      <c r="O11" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="P11" s="8" t="s">
+      <c r="P11" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="Q11" s="8" t="s">
+      <c r="Q11" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="R11" s="8" t="s">
+      <c r="R11" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="S11" s="8" t="s">
+      <c r="S11" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="T11" s="8" t="s">
+      <c r="T11" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="U11" s="8" t="s">
+      <c r="U11" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="V11" s="8" t="s">
+      <c r="V11" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="W11" s="8" t="s">
+      <c r="W11" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="X11" s="8" t="s">
+      <c r="X11" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="Y11" s="8" t="s">
+      <c r="Y11" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="Z11" s="8" t="s">
+      <c r="Z11" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="AA11" s="8" t="s">
+      <c r="AA11" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="AB11" s="8" t="s">
+      <c r="AB11" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="AC11" s="8" t="s">
+      <c r="AC11" s="7" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="12" spans="3:38" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="M12" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="N12" s="8" t="s">
+      <c r="N12" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="O12" s="8" t="s">
+      <c r="O12" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="P12" s="8" t="s">
+      <c r="P12" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="Q12" s="8" t="s">
+      <c r="Q12" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="R12" s="8" t="s">
+      <c r="R12" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="S12" s="8" t="s">
+      <c r="S12" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="T12" s="8" t="s">
+      <c r="T12" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="U12" s="8" t="s">
+      <c r="U12" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="V12" s="8" t="s">
+      <c r="V12" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="W12" s="8" t="s">
+      <c r="W12" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="X12" s="8" t="s">
+      <c r="X12" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="Y12" s="8" t="s">
+      <c r="Y12" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="Z12" s="8" t="s">
+      <c r="Z12" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="AA12" s="8" t="s">
+      <c r="AA12" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="AB12" s="8" t="s">
+      <c r="AB12" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="AC12" s="8" t="s">
+      <c r="AC12" s="7" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="13" spans="3:38" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="L13" s="8" t="s">
+      <c r="L13" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="M13" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="N13" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="O13" s="8" t="s">
+      <c r="O13" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="Q13" s="8" t="s">
+      <c r="Q13" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="R13" s="8" t="s">
+      <c r="R13" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="S13" s="8" t="s">
+      <c r="S13" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="T13" s="8" t="s">
+      <c r="T13" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="U13" s="8" t="s">
+      <c r="U13" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="V13" s="8" t="s">
+      <c r="V13" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="W13" s="8" t="s">
+      <c r="W13" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="X13" s="8" t="s">
+      <c r="X13" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="Y13" s="8" t="s">
+      <c r="Y13" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="Z13" s="8" t="s">
+      <c r="Z13" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="AA13" s="8" t="s">
+      <c r="AA13" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="AB13" s="8" t="s">
+      <c r="AB13" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="AC13" s="8" t="s">
+      <c r="AC13" s="7" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="14" spans="3:38" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="L14" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="M14" s="8" t="s">
+      <c r="M14" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="N14" s="8" t="s">
+      <c r="N14" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="O14" s="8" t="s">
+      <c r="O14" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="Q14" s="8" t="s">
+      <c r="Q14" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="R14" s="8" t="s">
+      <c r="R14" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="S14" s="8" t="s">
+      <c r="S14" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="T14" s="8" t="s">
+      <c r="T14" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="U14" s="8" t="s">
+      <c r="U14" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="V14" s="8" t="s">
+      <c r="V14" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="W14" s="8" t="s">
+      <c r="W14" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="X14" s="8" t="s">
+      <c r="X14" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="Y14" s="8" t="s">
+      <c r="Y14" s="7" t="s">
         <v>329</v>
       </c>
-      <c r="Z14" s="8" t="s">
+      <c r="Z14" s="7" t="s">
         <v>330</v>
       </c>
-      <c r="AA14" s="8" t="s">
+      <c r="AA14" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="AB14" s="8" t="s">
+      <c r="AB14" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="AC14" s="8" t="s">
+      <c r="AC14" s="7" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="15" spans="3:38" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="L15" s="8" t="s">
+      <c r="L15" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="M15" s="8" t="s">
+      <c r="M15" s="7" t="s">
         <v>344</v>
       </c>
-      <c r="N15" s="8" t="s">
+      <c r="N15" s="7" t="s">
         <v>345</v>
       </c>
-      <c r="O15" s="8" t="s">
+      <c r="O15" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="Q15" s="8" t="s">
+      <c r="Q15" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="R15" s="8" t="s">
+      <c r="R15" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="S15" s="8" t="s">
+      <c r="S15" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="T15" s="8" t="s">
+      <c r="T15" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="U15" s="8" t="s">
+      <c r="U15" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="V15" s="8" t="s">
+      <c r="V15" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="W15" s="8" t="s">
+      <c r="W15" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="X15" s="8" t="s">
+      <c r="X15" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="Y15" s="8" t="s">
+      <c r="Y15" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="Z15" s="8" t="s">
+      <c r="Z15" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="AA15" s="8" t="s">
+      <c r="AA15" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="AB15" s="8" t="s">
+      <c r="AB15" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="AC15" s="8" t="s">
+      <c r="AC15" s="7" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="16" spans="3:38" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="L16" s="8" t="s">
+      <c r="L16" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="M16" s="8" t="s">
+      <c r="M16" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="N16" s="8" t="s">
+      <c r="N16" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="O16" s="8" t="s">
+      <c r="O16" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="Q16" s="8" t="s">
+      <c r="Q16" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="R16" s="8" t="s">
+      <c r="R16" s="7" t="s">
         <v>373</v>
       </c>
-      <c r="S16" s="8" t="s">
+      <c r="S16" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="T16" s="8" t="s">
+      <c r="T16" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="U16" s="8" t="s">
+      <c r="U16" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="V16" s="8" t="s">
+      <c r="V16" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="W16" s="8" t="s">
+      <c r="W16" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="Y16" s="8" t="s">
+      <c r="Y16" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="Z16" s="8" t="s">
+      <c r="Z16" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="AA16" s="8" t="s">
+      <c r="AA16" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="AB16" s="8" t="s">
+      <c r="AB16" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="AC16" s="8" t="s">
+      <c r="AC16" s="7" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="17" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="K17" s="7" t="s">
         <v>392</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="L17" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="M17" s="8" t="s">
+      <c r="M17" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="N17" s="8" t="s">
+      <c r="N17" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="O17" s="8" t="s">
+      <c r="O17" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="Q17" s="8" t="s">
+      <c r="Q17" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="R17" s="8" t="s">
+      <c r="R17" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="S17" s="8" t="s">
+      <c r="S17" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="T17" s="8" t="s">
+      <c r="T17" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="U17" s="8" t="s">
+      <c r="U17" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="V17" s="8" t="s">
+      <c r="V17" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="W17" s="8" t="s">
+      <c r="W17" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="Y17" s="8" t="s">
+      <c r="Y17" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="Z17" s="8" t="s">
+      <c r="Z17" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="AC17" s="8" t="s">
+      <c r="AC17" s="7" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="18" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J18" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K18" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="L18" s="8" t="s">
+      <c r="L18" s="7" t="s">
         <v>416</v>
       </c>
-      <c r="N18" s="8" t="s">
+      <c r="N18" s="7" t="s">
         <v>417</v>
       </c>
-      <c r="O18" s="8" t="s">
+      <c r="O18" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="Q18" s="8" t="s">
+      <c r="Q18" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="R18" s="8" t="s">
+      <c r="R18" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="S18" s="8" t="s">
+      <c r="S18" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="T18" s="8" t="s">
+      <c r="T18" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="U18" s="8" t="s">
+      <c r="U18" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="V18" s="8" t="s">
+      <c r="V18" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="W18" s="8" t="s">
+      <c r="W18" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="Y18" s="8" t="s">
+      <c r="Y18" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="Z18" s="8" t="s">
+      <c r="Z18" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="AC18" s="8" t="s">
+      <c r="AC18" s="7" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="19" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="7" t="s">
         <v>432</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="7" t="s">
         <v>434</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K19" s="7" t="s">
         <v>436</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="L19" s="7" t="s">
         <v>437</v>
       </c>
-      <c r="N19" s="8" t="s">
+      <c r="N19" s="7" t="s">
         <v>438</v>
       </c>
-      <c r="O19" s="8" t="s">
+      <c r="O19" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="Q19" s="8" t="s">
+      <c r="Q19" s="7" t="s">
         <v>440</v>
       </c>
-      <c r="R19" s="8" t="s">
+      <c r="R19" s="7" t="s">
         <v>441</v>
       </c>
-      <c r="S19" s="8" t="s">
+      <c r="S19" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="T19" s="8" t="s">
+      <c r="T19" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="U19" s="8" t="s">
+      <c r="U19" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="V19" s="8" t="s">
+      <c r="V19" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="W19" s="8" t="s">
+      <c r="W19" s="7" t="s">
         <v>446</v>
       </c>
-      <c r="Y19" s="8" t="s">
+      <c r="Y19" s="7" t="s">
         <v>447</v>
       </c>
-      <c r="Z19" s="8" t="s">
+      <c r="Z19" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="AC19" s="8" t="s">
+      <c r="AC19" s="7" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="20" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>451</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="7" t="s">
         <v>454</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="K20" s="7" t="s">
         <v>457</v>
       </c>
-      <c r="L20" s="8" t="s">
+      <c r="L20" s="7" t="s">
         <v>458</v>
       </c>
-      <c r="N20" s="8" t="s">
+      <c r="N20" s="7" t="s">
         <v>459</v>
       </c>
-      <c r="O20" s="8" t="s">
+      <c r="O20" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="Q20" s="8" t="s">
+      <c r="Q20" s="7" t="s">
         <v>461</v>
       </c>
-      <c r="R20" s="8" t="s">
+      <c r="R20" s="7" t="s">
         <v>462</v>
       </c>
-      <c r="S20" s="8" t="s">
+      <c r="S20" s="7" t="s">
         <v>463</v>
       </c>
-      <c r="T20" s="8" t="s">
+      <c r="T20" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="U20" s="8" t="s">
+      <c r="U20" s="7" t="s">
         <v>465</v>
       </c>
-      <c r="V20" s="8" t="s">
+      <c r="V20" s="7" t="s">
         <v>466</v>
       </c>
-      <c r="Y20" s="8" t="s">
+      <c r="Y20" s="7" t="s">
         <v>467</v>
       </c>
-      <c r="Z20" s="8" t="s">
+      <c r="Z20" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="AC20" s="8" t="s">
+      <c r="AC20" s="7" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="21" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="7" t="s">
         <v>472</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="7" t="s">
         <v>473</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="7" t="s">
         <v>474</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J21" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K21" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="L21" s="8" t="s">
+      <c r="L21" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="O21" s="8" t="s">
+      <c r="O21" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="Q21" s="8" t="s">
+      <c r="Q21" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="R21" s="8" t="s">
+      <c r="R21" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="S21" s="8" t="s">
+      <c r="S21" s="7" t="s">
         <v>482</v>
       </c>
-      <c r="T21" s="8" t="s">
+      <c r="T21" s="7" t="s">
         <v>483</v>
       </c>
-      <c r="U21" s="8" t="s">
+      <c r="U21" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="V21" s="8" t="s">
+      <c r="V21" s="7" t="s">
         <v>485</v>
       </c>
-      <c r="Y21" s="8" t="s">
+      <c r="Y21" s="7" t="s">
         <v>486</v>
       </c>
-      <c r="Z21" s="8" t="s">
+      <c r="Z21" s="7" t="s">
         <v>487</v>
       </c>
-      <c r="AC21" s="8" t="s">
+      <c r="AC21" s="7" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="22" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>489</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>490</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>493</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="7" t="s">
         <v>494</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="7" t="s">
         <v>495</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="K22" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="L22" s="8" t="s">
+      <c r="L22" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="O22" s="8" t="s">
+      <c r="O22" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="Q22" s="8" t="s">
+      <c r="Q22" s="7" t="s">
         <v>499</v>
       </c>
-      <c r="R22" s="8" t="s">
+      <c r="R22" s="7" t="s">
         <v>500</v>
       </c>
-      <c r="S22" s="8" t="s">
+      <c r="S22" s="7" t="s">
         <v>501</v>
       </c>
-      <c r="T22" s="8" t="s">
+      <c r="T22" s="7" t="s">
         <v>502</v>
       </c>
-      <c r="U22" s="8" t="s">
+      <c r="U22" s="7" t="s">
         <v>503</v>
       </c>
-      <c r="V22" s="8" t="s">
+      <c r="V22" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="Y22" s="8" t="s">
+      <c r="Y22" s="7" t="s">
         <v>505</v>
       </c>
-      <c r="Z22" s="8" t="s">
+      <c r="Z22" s="7" t="s">
         <v>506</v>
       </c>
-      <c r="AC22" s="8" t="s">
+      <c r="AC22" s="7" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="23" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>508</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="7" t="s">
         <v>509</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="7" t="s">
         <v>510</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="7" t="s">
         <v>511</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="7" t="s">
         <v>512</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="7" t="s">
         <v>513</v>
       </c>
-      <c r="J23" s="8" t="s">
+      <c r="J23" s="7" t="s">
         <v>514</v>
       </c>
-      <c r="K23" s="8" t="s">
+      <c r="K23" s="7" t="s">
         <v>515</v>
       </c>
-      <c r="L23" s="8" t="s">
+      <c r="L23" s="7" t="s">
         <v>516</v>
       </c>
-      <c r="O23" s="8" t="s">
+      <c r="O23" s="7" t="s">
         <v>517</v>
       </c>
-      <c r="Q23" s="8" t="s">
+      <c r="Q23" s="7" t="s">
         <v>518</v>
       </c>
-      <c r="R23" s="8" t="s">
+      <c r="R23" s="7" t="s">
         <v>519</v>
       </c>
-      <c r="S23" s="8" t="s">
+      <c r="S23" s="7" t="s">
         <v>520</v>
       </c>
-      <c r="T23" s="8" t="s">
+      <c r="T23" s="7" t="s">
         <v>521</v>
       </c>
-      <c r="U23" s="8" t="s">
+      <c r="U23" s="7" t="s">
         <v>522</v>
       </c>
-      <c r="V23" s="8" t="s">
+      <c r="V23" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="Y23" s="8" t="s">
+      <c r="Y23" s="7" t="s">
         <v>524</v>
       </c>
-      <c r="Z23" s="8" t="s">
+      <c r="Z23" s="7" t="s">
         <v>525</v>
       </c>
-      <c r="AC23" s="8" t="s">
+      <c r="AC23" s="7" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="24" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>527</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>528</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="7" t="s">
         <v>529</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="7" t="s">
         <v>530</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="H24" s="7" t="s">
         <v>531</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="7" t="s">
         <v>532</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="J24" s="7" t="s">
         <v>533</v>
       </c>
-      <c r="K24" s="8" t="s">
+      <c r="K24" s="7" t="s">
         <v>534</v>
       </c>
-      <c r="L24" s="8" t="s">
+      <c r="L24" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="O24" s="8" t="s">
+      <c r="O24" s="7" t="s">
         <v>536</v>
       </c>
-      <c r="Q24" s="8" t="s">
+      <c r="Q24" s="7" t="s">
         <v>537</v>
       </c>
-      <c r="R24" s="8" t="s">
+      <c r="R24" s="7" t="s">
         <v>538</v>
       </c>
-      <c r="S24" s="8" t="s">
+      <c r="S24" s="7" t="s">
         <v>539</v>
       </c>
-      <c r="T24" s="8" t="s">
+      <c r="T24" s="7" t="s">
         <v>540</v>
       </c>
-      <c r="U24" s="8" t="s">
+      <c r="U24" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="V24" s="8" t="s">
+      <c r="V24" s="7" t="s">
         <v>542</v>
       </c>
-      <c r="Y24" s="8" t="s">
+      <c r="Y24" s="7" t="s">
         <v>543</v>
       </c>
-      <c r="Z24" s="8" t="s">
+      <c r="Z24" s="7" t="s">
         <v>544</v>
       </c>
-      <c r="AC24" s="8" t="s">
+      <c r="AC24" s="7" t="s">
         <v>545</v>
       </c>
     </row>
     <row r="25" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>546</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>547</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="7" t="s">
         <v>548</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="7" t="s">
         <v>549</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="7" t="s">
         <v>550</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J25" s="7" t="s">
         <v>551</v>
       </c>
-      <c r="K25" s="8" t="s">
+      <c r="K25" s="7" t="s">
         <v>552</v>
       </c>
-      <c r="L25" s="8" t="s">
+      <c r="L25" s="7" t="s">
         <v>553</v>
       </c>
-      <c r="O25" s="8" t="s">
+      <c r="O25" s="7" t="s">
         <v>554</v>
       </c>
-      <c r="R25" s="8" t="s">
+      <c r="R25" s="7" t="s">
         <v>555</v>
       </c>
-      <c r="S25" s="8" t="s">
+      <c r="S25" s="7" t="s">
         <v>556</v>
       </c>
-      <c r="T25" s="8" t="s">
+      <c r="T25" s="7" t="s">
         <v>557</v>
       </c>
-      <c r="U25" s="8" t="s">
+      <c r="U25" s="7" t="s">
         <v>558</v>
       </c>
-      <c r="V25" s="8" t="s">
+      <c r="V25" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="Y25" s="8" t="s">
+      <c r="Y25" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="Z25" s="8" t="s">
+      <c r="Z25" s="7" t="s">
         <v>561</v>
       </c>
-      <c r="AC25" s="8" t="s">
+      <c r="AC25" s="7" t="s">
         <v>562</v>
       </c>
     </row>
     <row r="26" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>563</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="7" t="s">
         <v>564</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
         <v>565</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="7" t="s">
         <v>566</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H26" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="J26" s="7" t="s">
         <v>568</v>
       </c>
-      <c r="K26" s="8" t="s">
+      <c r="K26" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="L26" s="8" t="s">
+      <c r="L26" s="7" t="s">
         <v>570</v>
       </c>
-      <c r="O26" s="8" t="s">
+      <c r="O26" s="7" t="s">
         <v>571</v>
       </c>
-      <c r="R26" s="8" t="s">
+      <c r="R26" s="7" t="s">
         <v>572</v>
       </c>
-      <c r="S26" s="8" t="s">
+      <c r="S26" s="7" t="s">
         <v>573</v>
       </c>
-      <c r="T26" s="8" t="s">
+      <c r="T26" s="7" t="s">
         <v>574</v>
       </c>
-      <c r="U26" s="8" t="s">
+      <c r="U26" s="7" t="s">
         <v>575</v>
       </c>
-      <c r="V26" s="8" t="s">
+      <c r="V26" s="7" t="s">
         <v>576</v>
       </c>
-      <c r="Y26" s="8" t="s">
+      <c r="Y26" s="7" t="s">
         <v>577</v>
       </c>
-      <c r="Z26" s="8" t="s">
+      <c r="Z26" s="7" t="s">
         <v>578</v>
       </c>
-      <c r="AC26" s="8" t="s">
+      <c r="AC26" s="7" t="s">
         <v>579</v>
       </c>
     </row>
     <row r="27" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>580</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="7" t="s">
         <v>581</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="7" t="s">
         <v>582</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="7" t="s">
         <v>583</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="7" t="s">
         <v>584</v>
       </c>
-      <c r="J27" s="8" t="s">
+      <c r="J27" s="7" t="s">
         <v>585</v>
       </c>
-      <c r="K27" s="8" t="s">
+      <c r="K27" s="7" t="s">
         <v>586</v>
       </c>
-      <c r="L27" s="8" t="s">
+      <c r="L27" s="7" t="s">
         <v>587</v>
       </c>
-      <c r="O27" s="8" t="s">
+      <c r="O27" s="7" t="s">
         <v>588</v>
       </c>
-      <c r="R27" s="8" t="s">
+      <c r="R27" s="7" t="s">
         <v>589</v>
       </c>
-      <c r="S27" s="8" t="s">
+      <c r="S27" s="7" t="s">
         <v>590</v>
       </c>
-      <c r="T27" s="8" t="s">
+      <c r="T27" s="7" t="s">
         <v>591</v>
       </c>
-      <c r="V27" s="8" t="s">
+      <c r="V27" s="7" t="s">
         <v>592</v>
       </c>
-      <c r="Y27" s="8" t="s">
+      <c r="Y27" s="7" t="s">
         <v>593</v>
       </c>
-      <c r="Z27" s="8" t="s">
+      <c r="Z27" s="7" t="s">
         <v>594</v>
       </c>
-      <c r="AC27" s="8" t="s">
+      <c r="AC27" s="7" t="s">
         <v>595</v>
       </c>
     </row>
     <row r="28" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="7" t="s">
         <v>596</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="7" t="s">
         <v>597</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="7" t="s">
         <v>598</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="H28" s="7" t="s">
         <v>599</v>
       </c>
-      <c r="J28" s="8" t="s">
+      <c r="J28" s="7" t="s">
         <v>600</v>
       </c>
-      <c r="K28" s="8" t="s">
+      <c r="K28" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="L28" s="8" t="s">
+      <c r="L28" s="7" t="s">
         <v>602</v>
       </c>
-      <c r="O28" s="8" t="s">
+      <c r="O28" s="7" t="s">
         <v>603</v>
       </c>
-      <c r="R28" s="8" t="s">
+      <c r="R28" s="7" t="s">
         <v>604</v>
       </c>
-      <c r="S28" s="8" t="s">
+      <c r="S28" s="7" t="s">
         <v>605</v>
       </c>
-      <c r="T28" s="8" t="s">
+      <c r="T28" s="7" t="s">
         <v>606</v>
       </c>
-      <c r="V28" s="8" t="s">
+      <c r="V28" s="7" t="s">
         <v>607</v>
       </c>
-      <c r="Y28" s="8" t="s">
+      <c r="Y28" s="7" t="s">
         <v>608</v>
       </c>
-      <c r="Z28" s="8" t="s">
+      <c r="Z28" s="7" t="s">
         <v>609</v>
       </c>
-      <c r="AC28" s="8" t="s">
+      <c r="AC28" s="7" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="29" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>611</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="7" t="s">
         <v>612</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="7" t="s">
         <v>613</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H29" s="7" t="s">
         <v>614</v>
       </c>
-      <c r="J29" s="8" t="s">
+      <c r="J29" s="7" t="s">
         <v>615</v>
       </c>
-      <c r="K29" s="8" t="s">
+      <c r="K29" s="7" t="s">
         <v>616</v>
       </c>
-      <c r="L29" s="8" t="s">
+      <c r="L29" s="7" t="s">
         <v>617</v>
       </c>
-      <c r="O29" s="8" t="s">
+      <c r="O29" s="7" t="s">
         <v>618</v>
       </c>
-      <c r="R29" s="8" t="s">
+      <c r="R29" s="7" t="s">
         <v>619</v>
       </c>
-      <c r="S29" s="8" t="s">
+      <c r="S29" s="7" t="s">
         <v>620</v>
       </c>
-      <c r="V29" s="8" t="s">
+      <c r="V29" s="7" t="s">
         <v>621</v>
       </c>
-      <c r="Y29" s="8" t="s">
+      <c r="Y29" s="7" t="s">
         <v>622</v>
       </c>
-      <c r="Z29" s="8" t="s">
+      <c r="Z29" s="7" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="30" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>624</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="7" t="s">
         <v>625</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G30" s="7" t="s">
         <v>626</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="7" t="s">
         <v>627</v>
       </c>
-      <c r="J30" s="8" t="s">
+      <c r="J30" s="7" t="s">
         <v>628</v>
       </c>
-      <c r="K30" s="8" t="s">
+      <c r="K30" s="7" t="s">
         <v>629</v>
       </c>
-      <c r="L30" s="8" t="s">
+      <c r="L30" s="7" t="s">
         <v>630</v>
       </c>
-      <c r="O30" s="8" t="s">
+      <c r="O30" s="7" t="s">
         <v>631</v>
       </c>
-      <c r="R30" s="8" t="s">
+      <c r="R30" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="S30" s="8" t="s">
+      <c r="S30" s="7" t="s">
         <v>632</v>
       </c>
-      <c r="V30" s="8" t="s">
+      <c r="V30" s="7" t="s">
         <v>633</v>
       </c>
-      <c r="Y30" s="8" t="s">
+      <c r="Y30" s="7" t="s">
         <v>634</v>
       </c>
-      <c r="Z30" s="8" t="s">
+      <c r="Z30" s="7" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="31" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>636</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="7" t="s">
         <v>637</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G31" s="7" t="s">
         <v>638</v>
       </c>
-      <c r="J31" s="8" t="s">
+      <c r="J31" s="7" t="s">
         <v>639</v>
       </c>
-      <c r="K31" s="8" t="s">
+      <c r="K31" s="7" t="s">
         <v>640</v>
       </c>
-      <c r="L31" s="8" t="s">
+      <c r="L31" s="7" t="s">
         <v>641</v>
       </c>
-      <c r="O31" s="8" t="s">
+      <c r="O31" s="7" t="s">
         <v>642</v>
       </c>
-      <c r="R31" s="8" t="s">
+      <c r="R31" s="7" t="s">
         <v>643</v>
       </c>
-      <c r="S31" s="8" t="s">
+      <c r="S31" s="7" t="s">
         <v>644</v>
       </c>
-      <c r="V31" s="8" t="s">
+      <c r="V31" s="7" t="s">
         <v>645</v>
       </c>
-      <c r="Y31" s="8" t="s">
+      <c r="Y31" s="7" t="s">
         <v>646</v>
       </c>
-      <c r="Z31" s="8" t="s">
+      <c r="Z31" s="7" t="s">
         <v>647</v>
       </c>
     </row>
     <row r="32" spans="3:29" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>648</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="7" t="s">
         <v>649</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="7" t="s">
         <v>650</v>
       </c>
-      <c r="J32" s="8" t="s">
+      <c r="J32" s="7" t="s">
         <v>651</v>
       </c>
-      <c r="K32" s="8" t="s">
+      <c r="K32" s="7" t="s">
         <v>652</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="L32" s="7" t="s">
         <v>653</v>
       </c>
-      <c r="O32" s="8" t="s">
+      <c r="O32" s="7" t="s">
         <v>654</v>
       </c>
-      <c r="R32" s="8" t="s">
+      <c r="R32" s="7" t="s">
         <v>655</v>
       </c>
-      <c r="S32" s="8" t="s">
+      <c r="S32" s="7" t="s">
         <v>656</v>
       </c>
-      <c r="V32" s="8" t="s">
+      <c r="V32" s="7" t="s">
         <v>657</v>
       </c>
-      <c r="Z32" s="8" t="s">
+      <c r="Z32" s="7" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="33" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>659</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="7" t="s">
         <v>660</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" s="7" t="s">
         <v>661</v>
       </c>
-      <c r="J33" s="8" t="s">
+      <c r="J33" s="7" t="s">
         <v>662</v>
       </c>
-      <c r="K33" s="8" t="s">
+      <c r="K33" s="7" t="s">
         <v>663</v>
       </c>
-      <c r="L33" s="8" t="s">
+      <c r="L33" s="7" t="s">
         <v>664</v>
       </c>
-      <c r="R33" s="8" t="s">
+      <c r="R33" s="7" t="s">
         <v>665</v>
       </c>
-      <c r="S33" s="8" t="s">
+      <c r="S33" s="7" t="s">
         <v>666</v>
       </c>
-      <c r="V33" s="8" t="s">
+      <c r="V33" s="7" t="s">
         <v>667</v>
       </c>
-      <c r="Z33" s="8" t="s">
+      <c r="Z33" s="7" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="34" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="7" t="s">
         <v>669</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="7" t="s">
         <v>670</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="J34" s="8" t="s">
+      <c r="J34" s="7" t="s">
         <v>672</v>
       </c>
-      <c r="K34" s="8" t="s">
+      <c r="K34" s="7" t="s">
         <v>673</v>
       </c>
-      <c r="L34" s="8" t="s">
+      <c r="L34" s="7" t="s">
         <v>674</v>
       </c>
-      <c r="R34" s="8" t="s">
+      <c r="R34" s="7" t="s">
         <v>675</v>
       </c>
-      <c r="S34" s="8" t="s">
+      <c r="S34" s="7" t="s">
         <v>676</v>
       </c>
-      <c r="V34" s="8" t="s">
+      <c r="V34" s="7" t="s">
         <v>677</v>
       </c>
-      <c r="Z34" s="8" t="s">
+      <c r="Z34" s="7" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="35" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>679</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="7" t="s">
         <v>680</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G35" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J35" s="7" t="s">
         <v>681</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K35" s="7" t="s">
         <v>682</v>
       </c>
-      <c r="L35" s="8" t="s">
+      <c r="L35" s="7" t="s">
         <v>683</v>
       </c>
-      <c r="R35" s="8" t="s">
+      <c r="R35" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="S35" s="8" t="s">
+      <c r="S35" s="7" t="s">
         <v>684</v>
       </c>
-      <c r="V35" s="8" t="s">
+      <c r="V35" s="7" t="s">
         <v>685</v>
       </c>
-      <c r="Z35" s="8" t="s">
+      <c r="Z35" s="7" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="36" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="7" t="s">
         <v>686</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="7" t="s">
         <v>687</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G36" s="7" t="s">
         <v>688</v>
       </c>
-      <c r="J36" s="8" t="s">
+      <c r="J36" s="7" t="s">
         <v>689</v>
       </c>
-      <c r="L36" s="8" t="s">
+      <c r="L36" s="7" t="s">
         <v>690</v>
       </c>
-      <c r="R36" s="8" t="s">
+      <c r="R36" s="7" t="s">
         <v>691</v>
       </c>
-      <c r="S36" s="8" t="s">
+      <c r="S36" s="7" t="s">
         <v>692</v>
       </c>
-      <c r="V36" s="8" t="s">
+      <c r="V36" s="7" t="s">
         <v>693</v>
       </c>
-      <c r="Z36" s="8" t="s">
+      <c r="Z36" s="7" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="37" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="7" t="s">
         <v>694</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="7" t="s">
         <v>695</v>
       </c>
-      <c r="G37" s="8" t="s">
+      <c r="G37" s="7" t="s">
         <v>696</v>
       </c>
-      <c r="J37" s="8" t="s">
+      <c r="J37" s="7" t="s">
         <v>697</v>
       </c>
-      <c r="L37" s="8" t="s">
+      <c r="L37" s="7" t="s">
         <v>698</v>
       </c>
-      <c r="R37" s="8" t="s">
+      <c r="R37" s="7" t="s">
         <v>699</v>
       </c>
-      <c r="V37" s="8" t="s">
+      <c r="V37" s="7" t="s">
         <v>700</v>
       </c>
-      <c r="Z37" s="8" t="s">
+      <c r="Z37" s="7" t="s">
         <v>701</v>
       </c>
     </row>
     <row r="38" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="7" t="s">
         <v>702</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="7" t="s">
         <v>703</v>
       </c>
-      <c r="G38" s="8" t="s">
+      <c r="G38" s="7" t="s">
         <v>704</v>
       </c>
-      <c r="J38" s="8" t="s">
+      <c r="J38" s="7" t="s">
         <v>705</v>
       </c>
-      <c r="L38" s="8" t="s">
+      <c r="L38" s="7" t="s">
         <v>706</v>
       </c>
-      <c r="R38" s="8" t="s">
+      <c r="R38" s="7" t="s">
         <v>707</v>
       </c>
-      <c r="V38" s="8" t="s">
+      <c r="V38" s="7" t="s">
         <v>708</v>
       </c>
-      <c r="Z38" s="8" t="s">
+      <c r="Z38" s="7" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="39" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="7" t="s">
         <v>710</v>
       </c>
-      <c r="G39" s="8" t="s">
+      <c r="G39" s="7" t="s">
         <v>711</v>
       </c>
-      <c r="J39" s="8" t="s">
+      <c r="J39" s="7" t="s">
         <v>712</v>
       </c>
-      <c r="L39" s="8" t="s">
+      <c r="L39" s="7" t="s">
         <v>713</v>
       </c>
-      <c r="R39" s="8" t="s">
+      <c r="R39" s="7" t="s">
         <v>714</v>
       </c>
-      <c r="Z39" s="8" t="s">
+      <c r="Z39" s="7" t="s">
         <v>715</v>
       </c>
     </row>
     <row r="40" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="7" t="s">
         <v>716</v>
       </c>
-      <c r="G40" s="8" t="s">
+      <c r="G40" s="7" t="s">
         <v>717</v>
       </c>
-      <c r="J40" s="8" t="s">
+      <c r="J40" s="7" t="s">
         <v>718</v>
       </c>
-      <c r="L40" s="8" t="s">
+      <c r="L40" s="7" t="s">
         <v>719</v>
       </c>
-      <c r="R40" s="8" t="s">
+      <c r="R40" s="7" t="s">
         <v>720</v>
       </c>
-      <c r="Z40" s="8" t="s">
+      <c r="Z40" s="7" t="s">
         <v>721</v>
       </c>
     </row>
     <row r="41" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="7" t="s">
         <v>722</v>
       </c>
-      <c r="G41" s="8" t="s">
+      <c r="G41" s="7" t="s">
         <v>723</v>
       </c>
-      <c r="L41" s="8" t="s">
+      <c r="L41" s="7" t="s">
         <v>724</v>
       </c>
-      <c r="R41" s="8" t="s">
+      <c r="R41" s="7" t="s">
         <v>725</v>
       </c>
-      <c r="Z41" s="8" t="s">
+      <c r="Z41" s="7" t="s">
         <v>726</v>
       </c>
     </row>
     <row r="42" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="7" t="s">
         <v>727</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="G42" s="7" t="s">
         <v>728</v>
       </c>
-      <c r="L42" s="8" t="s">
+      <c r="L42" s="7" t="s">
         <v>729</v>
       </c>
-      <c r="R42" s="8" t="s">
+      <c r="R42" s="7" t="s">
         <v>730</v>
       </c>
-      <c r="Z42" s="8" t="s">
+      <c r="Z42" s="7" t="s">
         <v>731</v>
       </c>
     </row>
     <row r="43" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="7" t="s">
         <v>732</v>
       </c>
-      <c r="G43" s="8"/>
-      <c r="L43" s="8" t="s">
+      <c r="G43" s="7"/>
+      <c r="L43" s="7" t="s">
         <v>733</v>
       </c>
-      <c r="R43" s="8" t="s">
+      <c r="R43" s="7" t="s">
         <v>734</v>
       </c>
-      <c r="Z43" s="8" t="s">
+      <c r="Z43" s="7" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="44" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="7" t="s">
         <v>735</v>
       </c>
-      <c r="G44" s="8"/>
-      <c r="L44" s="8" t="s">
+      <c r="G44" s="7"/>
+      <c r="L44" s="7" t="s">
         <v>736</v>
       </c>
-      <c r="Z44" s="8" t="s">
+      <c r="Z44" s="7" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="45" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="7" t="s">
         <v>738</v>
       </c>
-      <c r="G45" s="8"/>
-      <c r="L45" s="8" t="s">
+      <c r="G45" s="7"/>
+      <c r="L45" s="7" t="s">
         <v>739</v>
       </c>
-      <c r="Z45" s="8" t="s">
+      <c r="Z45" s="7" t="s">
         <v>740</v>
       </c>
     </row>
     <row r="46" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="7" t="s">
         <v>741</v>
       </c>
-      <c r="G46" s="8"/>
-      <c r="L46" s="8" t="s">
+      <c r="G46" s="7"/>
+      <c r="L46" s="7" t="s">
         <v>742</v>
       </c>
-      <c r="Z46" s="8" t="s">
+      <c r="Z46" s="7" t="s">
         <v>743</v>
       </c>
     </row>
     <row r="47" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="7" t="s">
         <v>744</v>
       </c>
-      <c r="G47" s="8"/>
-      <c r="L47" s="8" t="s">
+      <c r="G47" s="7"/>
+      <c r="L47" s="7" t="s">
         <v>745</v>
       </c>
-      <c r="Z47" s="8" t="s">
+      <c r="Z47" s="7" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="48" spans="4:26" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="7" t="s">
         <v>747</v>
       </c>
-      <c r="G48" s="8"/>
-      <c r="L48" s="8" t="s">
+      <c r="G48" s="7"/>
+      <c r="L48" s="7" t="s">
         <v>748</v>
       </c>
-      <c r="Z48" s="8" t="s">
+      <c r="Z48" s="7" t="s">
         <v>749</v>
       </c>
     </row>
     <row r="49" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="7" t="s">
         <v>750</v>
       </c>
-      <c r="G49" s="8"/>
-      <c r="L49" s="8" t="s">
+      <c r="G49" s="7"/>
+      <c r="L49" s="7" t="s">
         <v>751</v>
       </c>
     </row>
     <row r="50" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="7" t="s">
         <v>752</v>
       </c>
-      <c r="G50" s="8"/>
-      <c r="L50" s="8" t="s">
+      <c r="G50" s="7"/>
+      <c r="L50" s="7" t="s">
         <v>753</v>
       </c>
     </row>
     <row r="51" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="7" t="s">
         <v>754</v>
       </c>
-      <c r="G51" s="8"/>
-      <c r="L51" s="8" t="s">
+      <c r="G51" s="7"/>
+      <c r="L51" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="52" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="7" t="s">
         <v>756</v>
       </c>
-      <c r="G52" s="8"/>
-      <c r="L52" s="8" t="s">
+      <c r="G52" s="7"/>
+      <c r="L52" s="7" t="s">
         <v>757</v>
       </c>
     </row>
     <row r="53" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="7" t="s">
         <v>758</v>
       </c>
-      <c r="G53" s="8"/>
-      <c r="L53" s="8" t="s">
+      <c r="G53" s="7"/>
+      <c r="L53" s="7" t="s">
         <v>759</v>
       </c>
     </row>
     <row r="54" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="7" t="s">
         <v>760</v>
       </c>
-      <c r="G54" s="8"/>
-      <c r="L54" s="8" t="s">
+      <c r="G54" s="7"/>
+      <c r="L54" s="7" t="s">
         <v>761</v>
       </c>
     </row>
     <row r="55" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D55" s="8" t="s">
+      <c r="D55" s="7" t="s">
         <v>762</v>
       </c>
-      <c r="G55" s="8"/>
-      <c r="L55" s="8" t="s">
+      <c r="G55" s="7"/>
+      <c r="L55" s="7" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="56" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D56" s="8" t="s">
+      <c r="D56" s="7" t="s">
         <v>764</v>
       </c>
-      <c r="G56" s="8"/>
-      <c r="L56" s="8" t="s">
+      <c r="G56" s="7"/>
+      <c r="L56" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="57" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D57" s="8" t="s">
+      <c r="D57" s="7" t="s">
         <v>765</v>
       </c>
-      <c r="G57" s="8"/>
-      <c r="L57" s="8" t="s">
+      <c r="G57" s="7"/>
+      <c r="L57" s="7" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="58" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D58" s="8" t="s">
+      <c r="D58" s="7" t="s">
         <v>767</v>
       </c>
-      <c r="G58" s="8"/>
-      <c r="L58" s="8" t="s">
+      <c r="G58" s="7"/>
+      <c r="L58" s="7" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="59" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D59" s="8" t="s">
+      <c r="D59" s="7" t="s">
         <v>769</v>
       </c>
-      <c r="G59" s="8"/>
-      <c r="L59" s="8" t="s">
+      <c r="G59" s="7"/>
+      <c r="L59" s="7" t="s">
         <v>770</v>
       </c>
     </row>
     <row r="60" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D60" s="8" t="s">
+      <c r="D60" s="7" t="s">
         <v>715</v>
       </c>
-      <c r="G60" s="8"/>
-      <c r="L60" s="8"/>
+      <c r="G60" s="7"/>
+      <c r="L60" s="7"/>
     </row>
     <row r="61" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D61" s="8" t="s">
+      <c r="D61" s="7" t="s">
         <v>771</v>
       </c>
-      <c r="G61" s="8"/>
-      <c r="L61" s="8"/>
+      <c r="G61" s="7"/>
+      <c r="L61" s="7"/>
     </row>
     <row r="62" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D62" s="8" t="s">
+      <c r="D62" s="7" t="s">
         <v>772</v>
       </c>
-      <c r="G62" s="8"/>
-      <c r="L62" s="8"/>
+      <c r="G62" s="7"/>
+      <c r="L62" s="7"/>
     </row>
     <row r="63" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D63" s="8" t="s">
+      <c r="D63" s="7" t="s">
         <v>773</v>
       </c>
-      <c r="G63" s="8"/>
-      <c r="L63" s="8"/>
+      <c r="G63" s="7"/>
+      <c r="L63" s="7"/>
     </row>
     <row r="64" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D64" s="8" t="s">
+      <c r="D64" s="7" t="s">
         <v>774</v>
       </c>
-      <c r="G64" s="8"/>
-      <c r="L64" s="8"/>
+      <c r="G64" s="7"/>
+      <c r="L64" s="7"/>
     </row>
     <row r="65" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D65" s="8" t="s">
+      <c r="D65" s="7" t="s">
         <v>775</v>
       </c>
-      <c r="G65" s="8"/>
-      <c r="L65" s="8"/>
+      <c r="G65" s="7"/>
+      <c r="L65" s="7"/>
     </row>
     <row r="66" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D66" s="8" t="s">
+      <c r="D66" s="7" t="s">
         <v>776</v>
       </c>
-      <c r="G66" s="8"/>
-      <c r="L66" s="8"/>
+      <c r="G66" s="7"/>
+      <c r="L66" s="7"/>
     </row>
     <row r="67" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D67" s="8" t="s">
+      <c r="D67" s="7" t="s">
         <v>777</v>
       </c>
-      <c r="G67" s="8"/>
-      <c r="L67" s="8"/>
+      <c r="G67" s="7"/>
+      <c r="L67" s="7"/>
     </row>
     <row r="68" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D68" s="8" t="s">
+      <c r="D68" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="G68" s="8"/>
-      <c r="L68" s="8"/>
+      <c r="G68" s="7"/>
+      <c r="L68" s="7"/>
     </row>
     <row r="69" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D69" s="8" t="s">
+      <c r="D69" s="7" t="s">
         <v>779</v>
       </c>
-      <c r="G69" s="8"/>
-      <c r="L69" s="8"/>
+      <c r="G69" s="7"/>
+      <c r="L69" s="7"/>
     </row>
     <row r="70" spans="4:12" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="D70" s="8" t="s">
+      <c r="D70" s="7" t="s">
         <v>780</v>
       </c>
-      <c r="G70" s="8"/>
-      <c r="L70" s="8"/>
+      <c r="G70" s="7"/>
+      <c r="L70" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>